<commit_message>
Logs and extent reports fixed.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwazinkosizwane\eclipse-workspace\takealot-automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B75A9FA-A832-4C69-88FE-0BABAD5F5703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7973514-C87C-48ED-8BF3-00A49ADE3198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="2148" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4920" yWindow="2148" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common info" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
-  <si>
-    <t>global_wait_time</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t>alert_wait_time</t>
   </si>
@@ -34,18 +31,6 @@
     <t>signup_page_title</t>
   </si>
   <si>
-    <t>STORE</t>
-  </si>
-  <si>
-    <t>login_page_title</t>
-  </si>
-  <si>
-    <t>product_category</t>
-  </si>
-  <si>
-    <t>phones</t>
-  </si>
-  <si>
     <t>kwazi</t>
   </si>
   <si>
@@ -194,6 +179,18 @@
   </si>
   <si>
     <t>empty-results-page</t>
+  </si>
+  <si>
+    <t>Takealot.com: Online Shopping | SA's leading online store</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>home_page_title</t>
   </si>
 </sst>
 </file>
@@ -574,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,43 +584,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>20</v>
+      <c r="A1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -635,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -647,119 +633,119 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -783,58 +769,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -858,50 +844,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Somewhat functional add to cart
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,29 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwazinkosizwane\eclipse-workspace\takealot-automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7973514-C87C-48ED-8BF3-00A49ADE3198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF05350B-8CDC-488C-BEFF-D8CD12C102EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="2148" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6876" yWindow="0" windowWidth="16260" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common info" sheetId="1" r:id="rId1"/>
     <sheet name="search data" sheetId="2" r:id="rId2"/>
     <sheet name="alert messages" sheetId="3" r:id="rId3"/>
     <sheet name="order form" sheetId="4" r:id="rId4"/>
+    <sheet name="products" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
   <si>
     <t>alert_wait_time</t>
   </si>
   <si>
-    <t>signup_page_title</t>
-  </si>
-  <si>
     <t>kwazi</t>
   </si>
   <si>
@@ -191,13 +203,115 @@
   </si>
   <si>
     <t>home_page_title</t>
+  </si>
+  <si>
+    <t>search_product</t>
+  </si>
+  <si>
+    <t>Execution Required</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Apple iPhone 15 Pro Max 256GB</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>VendorName</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>smartphones</t>
+  </si>
+  <si>
+    <t>Fujifilm Instax Mini 12 Camera + Case and Film</t>
+  </si>
+  <si>
+    <t>Fujifilm Instax</t>
+  </si>
+  <si>
+    <t>Cameras</t>
+  </si>
+  <si>
+    <t>Price®</t>
+  </si>
+  <si>
+    <t>Fender Squier SA-105CE Acoustic Electric Guitar</t>
+  </si>
+  <si>
+    <t>Squier</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Test CaseID</t>
+  </si>
+  <si>
+    <t>TC1</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Apex - Marine Luxury Men's Leather Watch</t>
+  </si>
+  <si>
+    <t>Apex</t>
+  </si>
+  <si>
+    <t>Watches and accessories</t>
+  </si>
+  <si>
+    <t>!/*][#$&amp;</t>
+  </si>
+  <si>
+    <t>cart_product</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +329,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -255,17 +384,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -571,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,18 +719,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -609,7 +743,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -619,134 +764,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -769,58 +954,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -844,53 +1029,246 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2300227-3FF8-4322-9A65-221530F0E639}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2">
+        <v>27595</v>
+      </c>
+      <c r="F2">
+        <v>4.8</v>
+      </c>
+      <c r="G2">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3">
+        <v>690</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>1999</v>
+      </c>
+      <c r="F4">
+        <v>4.8</v>
+      </c>
+      <c r="G4">
+        <v>120</v>
+      </c>
+      <c r="H4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5">
+        <v>3495</v>
+      </c>
+      <c r="F5">
+        <v>4.2</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39698B59-91B3-4E1C-9325-CF24E0A50812}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a Jenkinsfile and a readMe
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwazinkosizwane\eclipse-workspace\takealot-automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DF32B4-FB79-4431-8B1A-64E36D7863C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12FB0E4-C4B1-4365-9908-B8FE89F9D84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5616" yWindow="1728" windowWidth="17424" windowHeight="10212" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5616" yWindow="1728" windowWidth="17424" windowHeight="10212" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common info" sheetId="1" r:id="rId1"/>
     <sheet name="search data" sheetId="2" r:id="rId2"/>
     <sheet name="alert messages" sheetId="3" r:id="rId3"/>
     <sheet name="registration form" sheetId="4" r:id="rId4"/>
-    <sheet name="products" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
+    <sheet name="login form" sheetId="7" r:id="rId5"/>
+    <sheet name="products" sheetId="5" r:id="rId6"/>
+    <sheet name="test execution" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,14 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="122">
   <si>
     <t>alert_wait_time</t>
   </si>
   <si>
-    <t>kwazi</t>
-  </si>
-  <si>
     <t>invalid_username_alert</t>
   </si>
   <si>
@@ -304,9 +302,6 @@
     <t>TC001</t>
   </si>
   <si>
-    <t>john.doe@example.com</t>
-  </si>
-  <si>
     <t>P@ssw0rd</t>
   </si>
   <si>
@@ -349,9 +344,6 @@
     <t>Please enter your email address</t>
   </si>
   <si>
-    <t>john.doe@example</t>
-  </si>
-  <si>
     <t>Please enter a valid email address</t>
   </si>
   <si>
@@ -370,16 +362,49 @@
     <t>Please enter a 9 or 10-digit SA mobile number</t>
   </si>
   <si>
-    <t>recabo2313@brinkc.com</t>
-  </si>
-  <si>
-    <t>3ddddddd</t>
-  </si>
-  <si>
     <t>TC011</t>
   </si>
   <si>
-    <t>zwane</t>
+    <t>Mobile number must be at least 10 digits</t>
+  </si>
+  <si>
+    <t>012345679</t>
+  </si>
+  <si>
+    <t>012345680</t>
+  </si>
+  <si>
+    <t>012345681</t>
+  </si>
+  <si>
+    <t>012345682</t>
+  </si>
+  <si>
+    <t>012345683</t>
+  </si>
+  <si>
+    <t>012345684</t>
+  </si>
+  <si>
+    <t>012345</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>0612345678</t>
+  </si>
+  <si>
+    <t>john.doe@gmail.com</t>
+  </si>
+  <si>
+    <t>This email address is already registered on takealot.com</t>
+  </si>
+  <si>
+    <t>jon.doe@gmail.com</t>
+  </si>
+  <si>
+    <t>0612345679</t>
   </si>
 </sst>
 </file>
@@ -463,7 +488,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -477,10 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -805,18 +827,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -829,18 +851,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -865,154 +887,154 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
@@ -1039,58 +1061,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1100,297 +1122,340 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="61.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="G1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="C10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="F10" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="8">
-        <v>1234567890</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="D11" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1234567890</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1234567890</v>
-      </c>
-      <c r="G4" s="8" t="s">
+      <c r="D12" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1234567890</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" s="8">
-        <v>1234567890</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8">
-        <v>1234567890</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="8">
-        <v>1234567890</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F9" s="8">
-        <v>12345678</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="8">
-        <v>1234567892</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" s="8">
-        <v>1234567893</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" t="s">
-        <v>110</v>
-      </c>
-      <c r="E12" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" s="10">
-        <v>612345678</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{F40DAE33-E931-436D-BEC6-E0DD11B9ABAB}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0D529E-08E2-45D8-86EF-7CD9DFA7F38F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2300227-3FF8-4322-9A65-221530F0E639}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -1407,45 +1472,45 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2">
         <v>27595</v>
@@ -1457,24 +1522,24 @@
         <v>40</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
         <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>74</v>
       </c>
       <c r="E3">
         <v>690</v>
@@ -1486,24 +1551,24 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
         <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>61</v>
       </c>
       <c r="E4">
         <v>1999</v>
@@ -1515,24 +1580,24 @@
         <v>120</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
         <v>64</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
       </c>
       <c r="E5">
         <v>3495</v>
@@ -1544,10 +1609,10 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1556,12 +1621,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39698B59-91B3-4E1C-9325-CF24E0A50812}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1572,10 +1637,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login Test cases fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwazinkosizwane\eclipse-workspace\takealot-automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453BDB77-B39B-43EC-B8C7-7A53034CB3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EBD0B3-F6A8-47D4-A5F5-CBF4E1DFBA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5616" yWindow="1728" windowWidth="17424" windowHeight="10212" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1359,7 +1359,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>